<commit_message>
Exploratorio incial de encuesta
</commit_message>
<xml_diff>
--- a/_estadistica-descriptiva/basesdedatos/encuesta.xlsx
+++ b/_estadistica-descriptiva/basesdedatos/encuesta.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="55">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -157,12 +157,6 @@
     <t xml:space="preserve">Caminando</t>
   </si>
   <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
-  </si>
-  <si>
     <t xml:space="preserve">Estadistica</t>
   </si>
   <si>
@@ -172,7 +166,7 @@
     <t xml:space="preserve">Aero Vans </t>
   </si>
   <si>
-    <t xml:space="preserve">Bus </t>
+    <t xml:space="preserve">Bus</t>
   </si>
   <si>
     <t xml:space="preserve">Bicicleta</t>
@@ -187,9 +181,6 @@
     <t xml:space="preserve">Metroplus</t>
   </si>
   <si>
-    <t xml:space="preserve">Bus</t>
-  </si>
-  <si>
     <t xml:space="preserve">Carro</t>
   </si>
   <si>
@@ -197,12 +188,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ingenieria de Control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingenieria de Sistemas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
   </si>
 </sst>
 </file>
@@ -314,8 +299,8 @@
   </sheetPr>
   <dimension ref="A1:AH74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I75" activeCellId="0" sqref="I75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X5" activeCellId="0" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -323,19 +308,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="10.58"/>
@@ -343,12 +328,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="1" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="8.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="35" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="35" style="1" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -663,7 +648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
@@ -734,10 +719,10 @@
         <v>300</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="Z4" s="1" t="s">
         <v>39</v>
@@ -767,7 +752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
@@ -837,7 +822,7 @@
       <c r="W5" s="1" t="n">
         <v>1070</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="X5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="Y5" s="1" t="s">
@@ -882,7 +867,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>2</v>
@@ -918,7 +903,7 @@
         <v>55</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>36</v>
@@ -986,7 +971,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>2</v>
@@ -1022,7 +1007,7 @@
         <v>57</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q7" s="1" t="n">
         <v>4</v>
@@ -1079,7 +1064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
@@ -1126,7 +1111,7 @@
         <v>43</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q8" s="1" t="n">
         <v>5</v>
@@ -1230,7 +1215,7 @@
         <v>20</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q9" s="1" t="n">
         <v>4</v>
@@ -1298,7 +1283,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>2</v>
@@ -1334,7 +1319,7 @@
         <v>48</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q10" s="1" t="n">
         <v>3</v>
@@ -1402,7 +1387,7 @@
         <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>5</v>
@@ -1438,7 +1423,7 @@
         <v>7</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q11" s="1" t="n">
         <v>5</v>
@@ -1506,7 +1491,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>8</v>
@@ -1542,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q12" s="1" t="n">
         <v>5</v>
@@ -1646,7 +1631,7 @@
         <v>1</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q13" s="1" t="n">
         <v>5</v>
@@ -1750,7 +1735,7 @@
         <v>10</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q14" s="1" t="n">
         <v>5</v>
@@ -1854,7 +1839,7 @@
         <v>45</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q15" s="1" t="n">
         <v>5</v>
@@ -1922,7 +1907,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>2</v>
@@ -2015,7 +2000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
@@ -2062,7 +2047,7 @@
         <v>45</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q17" s="1" t="n">
         <v>5</v>
@@ -2270,7 +2255,7 @@
         <v>49</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q19" s="1" t="n">
         <v>5</v>
@@ -2374,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q20" s="1" t="n">
         <v>5</v>
@@ -2478,7 +2463,7 @@
         <v>49</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q21" s="1" t="n">
         <v>3</v>
@@ -2546,7 +2531,7 @@
         <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>2</v>
@@ -2650,7 +2635,7 @@
         <v>18</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" s="1" t="n">
         <v>2</v>
@@ -2686,7 +2671,7 @@
         <v>20</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q23" s="1" t="n">
         <v>4</v>
@@ -2754,7 +2739,7 @@
         <v>17</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E24" s="1" t="n">
         <v>2</v>
@@ -2858,7 +2843,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E25" s="1" t="n">
         <v>2</v>
@@ -2894,7 +2879,7 @@
         <v>53</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q25" s="1" t="n">
         <v>5</v>
@@ -2962,7 +2947,7 @@
         <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E26" s="1" t="n">
         <v>2</v>
@@ -2998,7 +2983,7 @@
         <v>30</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q26" s="1" t="n">
         <v>5</v>
@@ -3066,7 +3051,7 @@
         <v>18</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E27" s="1" t="n">
         <v>2</v>
@@ -3102,7 +3087,7 @@
         <v>20</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q27" s="1" t="n">
         <v>5</v>
@@ -3170,7 +3155,7 @@
         <v>17</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E28" s="1" t="n">
         <v>2</v>
@@ -3206,7 +3191,7 @@
         <v>34</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q28" s="1" t="n">
         <v>4</v>
@@ -3310,7 +3295,7 @@
         <v>47</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q29" s="1" t="n">
         <v>4</v>
@@ -3518,7 +3503,7 @@
         <v>17</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q31" s="1" t="n">
         <v>4</v>
@@ -3586,7 +3571,7 @@
         <v>19</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E32" s="1" t="n">
         <v>2</v>
@@ -3622,7 +3607,7 @@
         <v>55</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q32" s="1" t="n">
         <v>4</v>
@@ -3726,7 +3711,7 @@
         <v>51</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q33" s="1" t="n">
         <v>4</v>
@@ -3794,7 +3779,7 @@
         <v>19</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E34" s="1" t="n">
         <v>2</v>
@@ -3830,7 +3815,7 @@
         <v>48</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q34" s="1" t="n">
         <v>5</v>
@@ -3898,7 +3883,7 @@
         <v>23</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E35" s="1" t="n">
         <v>2</v>
@@ -3934,7 +3919,7 @@
         <v>5</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q35" s="1" t="n">
         <v>4</v>
@@ -4002,7 +3987,7 @@
         <v>17</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E36" s="1" t="n">
         <v>2</v>
@@ -4038,7 +4023,7 @@
         <v>10</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q36" s="1" t="n">
         <v>4</v>
@@ -4106,7 +4091,7 @@
         <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E37" s="1" t="n">
         <v>2</v>
@@ -4142,7 +4127,7 @@
         <v>35</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q37" s="1" t="n">
         <v>4</v>
@@ -4210,7 +4195,7 @@
         <v>17</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E38" s="1" t="n">
         <v>2</v>
@@ -4246,7 +4231,7 @@
         <v>52</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q38" s="1" t="n">
         <v>5</v>
@@ -4314,7 +4299,7 @@
         <v>17</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E39" s="1" t="n">
         <v>2</v>
@@ -4350,7 +4335,7 @@
         <v>50</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q39" s="1" t="n">
         <v>5</v>
@@ -4418,7 +4403,7 @@
         <v>17</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E40" s="1" t="n">
         <v>2</v>
@@ -4522,7 +4507,7 @@
         <v>22</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E41" s="1" t="n">
         <v>3</v>
@@ -4558,7 +4543,7 @@
         <v>5</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q41" s="1" t="n">
         <v>5</v>
@@ -4626,7 +4611,7 @@
         <v>17</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E42" s="1" t="n">
         <v>2</v>
@@ -4662,7 +4647,7 @@
         <v>53</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q42" s="1" t="n">
         <v>4</v>
@@ -4766,7 +4751,7 @@
         <v>52</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q43" s="1" t="n">
         <v>5</v>
@@ -4834,7 +4819,7 @@
         <v>17</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E44" s="1" t="n">
         <v>2</v>
@@ -4870,7 +4855,7 @@
         <v>8</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q44" s="1" t="n">
         <v>4</v>
@@ -4938,7 +4923,7 @@
         <v>18</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E45" s="1" t="n">
         <v>3</v>
@@ -4974,7 +4959,7 @@
         <v>50</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q45" s="1" t="n">
         <v>4</v>
@@ -5042,7 +5027,7 @@
         <v>17</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E46" s="1" t="n">
         <v>2</v>
@@ -5135,7 +5120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
@@ -5146,7 +5131,7 @@
         <v>24</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E47" s="1" t="n">
         <v>4</v>
@@ -5250,7 +5235,7 @@
         <v>17</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E48" s="1" t="n">
         <v>2</v>
@@ -5286,7 +5271,7 @@
         <v>2</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q48" s="1" t="n">
         <v>4</v>
@@ -5343,7 +5328,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>48</v>
       </c>
@@ -5354,7 +5339,7 @@
         <v>24</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E49" s="1" t="n">
         <v>4</v>
@@ -5390,7 +5375,7 @@
         <v>54</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q49" s="1" t="n">
         <v>4</v>
@@ -5447,7 +5432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
@@ -5458,7 +5443,7 @@
         <v>25</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E50" s="1" t="n">
         <v>2</v>
@@ -5494,7 +5479,7 @@
         <v>55</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q50" s="1" t="n">
         <v>4</v>
@@ -5551,7 +5536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <v>50</v>
       </c>
@@ -5562,7 +5547,7 @@
         <v>23</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E51" s="1" t="n">
         <v>4</v>
@@ -5598,7 +5583,7 @@
         <v>15</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q51" s="1" t="n">
         <v>4</v>
@@ -5655,7 +5640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>51</v>
       </c>
@@ -5666,7 +5651,7 @@
         <v>17</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E52" s="1" t="n">
         <v>2</v>
@@ -5702,7 +5687,7 @@
         <v>40</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q52" s="1" t="n">
         <v>4</v>
@@ -5759,7 +5744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>52</v>
       </c>
@@ -5770,7 +5755,7 @@
         <v>18</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E53" s="1" t="n">
         <v>2</v>
@@ -5806,7 +5791,7 @@
         <v>55</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q53" s="1" t="n">
         <v>4</v>
@@ -5863,7 +5848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>53</v>
       </c>
@@ -5874,7 +5859,7 @@
         <v>18</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E54" s="1" t="n">
         <v>2</v>
@@ -5910,7 +5895,7 @@
         <v>45</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q54" s="1" t="n">
         <v>5</v>
@@ -5967,7 +5952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>54</v>
       </c>
@@ -5978,7 +5963,7 @@
         <v>17</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E55" s="1" t="n">
         <v>2</v>
@@ -6014,7 +5999,7 @@
         <v>2</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q55" s="1" t="n">
         <v>5</v>
@@ -6071,7 +6056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>55</v>
       </c>
@@ -6082,7 +6067,7 @@
         <v>18</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E56" s="1" t="n">
         <v>2</v>
@@ -6118,7 +6103,7 @@
         <v>43</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q56" s="1" t="n">
         <v>5</v>
@@ -6175,7 +6160,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <v>56</v>
       </c>
@@ -6186,7 +6171,7 @@
         <v>20</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E57" s="1" t="n">
         <v>2</v>
@@ -6222,7 +6207,7 @@
         <v>42</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q57" s="1" t="n">
         <v>5</v>
@@ -6255,7 +6240,7 @@
         <v>39</v>
       </c>
       <c r="AA57" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="AB57" s="1" t="s">
         <v>39</v>
@@ -6279,7 +6264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
         <v>57</v>
       </c>
@@ -6290,7 +6275,7 @@
         <v>18</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E58" s="1" t="n">
         <v>3</v>
@@ -6326,7 +6311,7 @@
         <v>4</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q58" s="1" t="n">
         <v>3</v>
@@ -6383,7 +6368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
         <v>58</v>
       </c>
@@ -6394,7 +6379,7 @@
         <v>17</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E59" s="1" t="n">
         <v>2</v>
@@ -6430,7 +6415,7 @@
         <v>56</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q59" s="1" t="n">
         <v>3</v>
@@ -6487,7 +6472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
         <v>59</v>
       </c>
@@ -6498,7 +6483,7 @@
         <v>18</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E60" s="1" t="n">
         <v>2</v>
@@ -6534,7 +6519,7 @@
         <v>5</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q60" s="1" t="n">
         <v>3</v>
@@ -6591,7 +6576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <v>60</v>
       </c>
@@ -6638,7 +6623,7 @@
         <v>20</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q61" s="1" t="n">
         <v>5</v>
@@ -6695,7 +6680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
         <v>61</v>
       </c>
@@ -6706,7 +6691,7 @@
         <v>21</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E62" s="1" t="n">
         <v>2</v>
@@ -6742,7 +6727,7 @@
         <v>58</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q62" s="1" t="n">
         <v>6</v>
@@ -6799,7 +6784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
         <v>62</v>
       </c>
@@ -6846,7 +6831,7 @@
         <v>0</v>
       </c>
       <c r="P63" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q63" s="1" t="n">
         <v>5</v>
@@ -6903,7 +6888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
         <v>63</v>
       </c>
@@ -6914,7 +6899,7 @@
         <v>17</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E64" s="1" t="n">
         <v>2</v>
@@ -6950,7 +6935,7 @@
         <v>52</v>
       </c>
       <c r="P64" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q64" s="1" t="n">
         <v>4</v>
@@ -7007,7 +6992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
         <v>64</v>
       </c>
@@ -7018,7 +7003,7 @@
         <v>17</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E65" s="1" t="n">
         <v>2</v>
@@ -7054,7 +7039,7 @@
         <v>49</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q65" s="1" t="n">
         <v>5</v>
@@ -7111,7 +7096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
         <v>65</v>
       </c>
@@ -7122,7 +7107,7 @@
         <v>18</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E66" s="1" t="n">
         <v>2</v>
@@ -7158,7 +7143,7 @@
         <v>53</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q66" s="1" t="n">
         <v>5</v>
@@ -7215,7 +7200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
         <v>66</v>
       </c>
@@ -7226,7 +7211,7 @@
         <v>20</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E67" s="1" t="n">
         <v>5</v>
@@ -7262,7 +7247,7 @@
         <v>15</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q67" s="1" t="n">
         <v>6</v>
@@ -7319,7 +7304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
         <v>67</v>
       </c>
@@ -7330,7 +7315,7 @@
         <v>18</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E68" s="1" t="n">
         <v>4</v>
@@ -7366,7 +7351,7 @@
         <v>50</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q68" s="1" t="n">
         <v>5</v>
@@ -7423,7 +7408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
         <v>68</v>
       </c>
@@ -7434,7 +7419,7 @@
         <v>40</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E69" s="1" t="n">
         <v>2</v>
@@ -7470,7 +7455,7 @@
         <v>49</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q69" s="1" t="n">
         <v>3</v>
@@ -7527,7 +7512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
         <v>69</v>
       </c>
@@ -7538,7 +7523,7 @@
         <v>21</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E70" s="1" t="n">
         <v>3</v>
@@ -7574,7 +7559,7 @@
         <v>0</v>
       </c>
       <c r="P70" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q70" s="1" t="n">
         <v>5</v>
@@ -7631,7 +7616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
         <v>70</v>
       </c>
@@ -7642,7 +7627,7 @@
         <v>18</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E71" s="1" t="n">
         <v>2</v>
@@ -7678,7 +7663,7 @@
         <v>55</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q71" s="1" t="n">
         <v>4</v>
@@ -7735,7 +7720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
         <v>71</v>
       </c>
@@ -7746,7 +7731,7 @@
         <v>22</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E72" s="1" t="n">
         <v>3</v>
@@ -7782,7 +7767,7 @@
         <v>56</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q72" s="1" t="n">
         <v>5</v>
@@ -7839,7 +7824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
         <v>72</v>
       </c>
@@ -7850,7 +7835,7 @@
         <v>18</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E73" s="1" t="n">
         <v>3</v>
@@ -7886,7 +7871,7 @@
         <v>10</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q73" s="1" t="n">
         <v>3</v>
@@ -7943,7 +7928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
         <v>73</v>
       </c>
@@ -7954,7 +7939,7 @@
         <v>19</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E74" s="1" t="n">
         <v>3</v>
@@ -7990,7 +7975,7 @@
         <v>6</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q74" s="1" t="n">
         <v>3</v>

</xml_diff>